<commit_message>
🔄 MAJ automatique BRVM via GitHub Actions
</commit_message>
<xml_diff>
--- a/data/recommandations.xlsx
+++ b/data/recommandations.xlsx
@@ -475,13 +475,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D2" t="n">
-        <v>55388.69</v>
+        <v>56241.74</v>
       </c>
       <c r="E2" t="n">
-        <v>121.14</v>
+        <v>120.2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -499,13 +499,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" t="n">
-        <v>45335</v>
+        <v>46285</v>
       </c>
       <c r="E3" t="n">
-        <v>975</v>
+        <v>950</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -523,13 +523,13 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D4" t="n">
-        <v>42903.51</v>
+        <v>43571.11</v>
       </c>
       <c r="E4" t="n">
-        <v>665.4400000000001</v>
+        <v>667.6</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -547,10 +547,10 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" t="n">
-        <v>42185</v>
+        <v>43175</v>
       </c>
       <c r="E5" t="n">
         <v>990</v>
@@ -564,20 +564,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SAFCA CI</t>
+          <t>NEI-CEDA CI</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D6" t="n">
-        <v>42085</v>
+        <v>42620</v>
       </c>
       <c r="E6" t="n">
-        <v>800</v>
+        <v>730</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -588,20 +588,20 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NEI-CEDA CI</t>
+          <t>SAFCA CI</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D7" t="n">
-        <v>41890</v>
+        <v>42085</v>
       </c>
       <c r="E7" t="n">
-        <v>730</v>
+        <v>800</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -619,13 +619,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D8" t="n">
-        <v>37280</v>
+        <v>37885</v>
       </c>
       <c r="E8" t="n">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -643,13 +643,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D9" t="n">
-        <v>36380</v>
+        <v>36930</v>
       </c>
       <c r="E9" t="n">
-        <v>595</v>
+        <v>550</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -667,13 +667,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D10" t="n">
-        <v>31245</v>
+        <v>31750</v>
       </c>
       <c r="E10" t="n">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -691,13 +691,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" t="n">
-        <v>25260</v>
+        <v>25655</v>
       </c>
       <c r="E11" t="n">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -715,13 +715,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D12" t="n">
-        <v>23162.66</v>
+        <v>23542.77</v>
       </c>
       <c r="E12" t="n">
-        <v>380.19</v>
+        <v>380.11</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -739,13 +739,13 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D13" t="n">
-        <v>20798.21</v>
+        <v>21136.33</v>
       </c>
       <c r="E13" t="n">
-        <v>339.32</v>
+        <v>338.12</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -763,13 +763,13 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D14" t="n">
-        <v>13503.95</v>
+        <v>13737.75</v>
       </c>
       <c r="E14" t="n">
-        <v>231.28</v>
+        <v>233.8</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -787,13 +787,13 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D15" t="n">
-        <v>9243.889999999999</v>
+        <v>9400.35</v>
       </c>
       <c r="E15" t="n">
-        <v>156.64</v>
+        <v>156.46</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -811,13 +811,13 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" t="n">
-        <v>8277.129999999999</v>
+        <v>8416.41</v>
       </c>
       <c r="E16" t="n">
-        <v>138.11</v>
+        <v>139.28</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -835,13 +835,13 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" t="n">
-        <v>7624.76</v>
+        <v>7746.69</v>
       </c>
       <c r="E17" t="n">
-        <v>121.9</v>
+        <v>121.93</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -859,13 +859,13 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" t="n">
-        <v>7086.5</v>
+        <v>7206.16</v>
       </c>
       <c r="E18" t="n">
-        <v>118.38</v>
+        <v>119.66</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -883,13 +883,13 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D19" t="n">
-        <v>7016.11</v>
+        <v>7135.18</v>
       </c>
       <c r="E19" t="n">
-        <v>117.07</v>
+        <v>119.07</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -907,13 +907,13 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D20" t="n">
-        <v>6863.56</v>
+        <v>6980.1</v>
       </c>
       <c r="E20" t="n">
-        <v>116.7</v>
+        <v>116.54</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -931,13 +931,13 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D21" t="n">
-        <v>6767.94</v>
+        <v>6881.77</v>
       </c>
       <c r="E21" t="n">
-        <v>114.09</v>
+        <v>113.83</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -955,13 +955,13 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D22" t="n">
-        <v>6651.33</v>
+        <v>6763.2</v>
       </c>
       <c r="E22" t="n">
-        <v>112.13</v>
+        <v>111.87</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -979,13 +979,13 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D23" t="n">
-        <v>6324.86</v>
+        <v>6419.97</v>
       </c>
       <c r="E23" t="n">
-        <v>95.25</v>
+        <v>95.11</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1003,13 +1003,13 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D24" t="n">
-        <v>6261.46</v>
+        <v>6358.52</v>
       </c>
       <c r="E24" t="n">
-        <v>99.65000000000001</v>
+        <v>97.06</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1308,20 +1308,20 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CFAO MOTORS CI (CFAC)</t>
+          <t>SAFCA CI (SAFC)</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C37" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D37" t="n">
-        <v>23.04</v>
+        <v>22.3</v>
       </c>
       <c r="E37" t="n">
-        <v>6.14</v>
+        <v>1.27</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1332,20 +1332,20 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>SAFCA CI (SAFC)</t>
+          <t>PALM CI (PALC)</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>8</v>
       </c>
       <c r="C38" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D38" t="n">
-        <v>22.3</v>
+        <v>21.55</v>
       </c>
       <c r="E38" t="n">
-        <v>1.27</v>
+        <v>-4.17</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1356,20 +1356,20 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PALM CI (PALC)</t>
+          <t>BERNABE CI (BNBC)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C39" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D39" t="n">
-        <v>21.55</v>
+        <v>20.16</v>
       </c>
       <c r="E39" t="n">
-        <v>-4.17</v>
+        <v>6</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1380,20 +1380,20 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>BERNABE CI (BNBC)</t>
+          <t>CFAO MOTORS CI (CFAC)</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C40" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40" t="n">
-        <v>20.16</v>
+        <v>16.48</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>-6.56</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1452,20 +1452,20 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>SUCRIVOIRE (SCRC)</t>
+          <t>BANK OF AFRICA NG (BOAN)</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C43" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D43" t="n">
-        <v>13.77</v>
+        <v>13.55</v>
       </c>
       <c r="E43" t="n">
-        <v>2.04</v>
+        <v>4.49</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1476,20 +1476,20 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>BANK OF AFRICA NG (BOAN)</t>
+          <t>SUCRIVOIRE (SCRC)</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C44" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D44" t="n">
-        <v>13.55</v>
+        <v>12.76</v>
       </c>
       <c r="E44" t="n">
-        <v>4.49</v>
+        <v>-1.01</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -1507,13 +1507,13 @@
         <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D45" t="n">
-        <v>12.34</v>
+        <v>11.06</v>
       </c>
       <c r="E45" t="n">
-        <v>-3.04</v>
+        <v>-1.28</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -1579,13 +1579,13 @@
         <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D48" t="n">
-        <v>9.51</v>
+        <v>7.68</v>
       </c>
       <c r="E48" t="n">
-        <v>3.08</v>
+        <v>-1.83</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -1644,20 +1644,20 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>UNILEVER CI (UNLC)</t>
+          <t>VIVO ENERGY CI (SHEC)</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C51" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D51" t="n">
-        <v>2.53</v>
+        <v>2.92</v>
       </c>
       <c r="E51" t="n">
-        <v>-7.46</v>
+        <v>2.63</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -1668,20 +1668,20 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>SETAO CI (STAC)</t>
+          <t>UNILEVER CI (UNLC)</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C52" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D52" t="n">
-        <v>0.44</v>
+        <v>2.53</v>
       </c>
       <c r="E52" t="n">
-        <v>-6.84</v>
+        <v>-7.46</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -1692,20 +1692,20 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>VIVO ENERGY CI (SHEC)</t>
+          <t>SETAO CI (STAC)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C53" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D53" t="n">
-        <v>0.29</v>
+        <v>2.27</v>
       </c>
       <c r="E53" t="n">
-        <v>-2.56</v>
+        <v>1.83</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -1723,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -1788,20 +1788,20 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>SOCIETE GENERALE COTE D'IVOIRE (SGBC)</t>
+          <t>TOTALENERGIES MARKETING SN (TTLS)</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C57" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D57" t="n">
-        <v>-6.92</v>
+        <v>-6.43</v>
       </c>
       <c r="E57" t="n">
-        <v>-1.35</v>
+        <v>2.34</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -1812,20 +1812,20 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>TOTALENERGIES MARKETING SN (TTLS)</t>
+          <t>SOGB CI (SOGC)</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C58" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D58" t="n">
-        <v>-8.77</v>
+        <v>-6.54</v>
       </c>
       <c r="E58" t="n">
-        <v>-3.69</v>
+        <v>2.78</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -1836,20 +1836,20 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>LOTERIE NATIONALE DU BENIN (LNBB)</t>
+          <t>SOCIETE GENERALE COTE D'IVOIRE (SGBC)</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C59" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D59" t="n">
-        <v>-9.130000000000001</v>
+        <v>-6.92</v>
       </c>
       <c r="E59" t="n">
-        <v>-2.63</v>
+        <v>-1.35</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -1860,20 +1860,20 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>SOGB CI (SOGC)</t>
+          <t>LOTERIE NATIONALE DU BENIN (LNBB)</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C60" t="n">
         <v>5</v>
       </c>
       <c r="D60" t="n">
-        <v>-9.32</v>
+        <v>-9.130000000000001</v>
       </c>
       <c r="E60" t="n">
-        <v>0.83</v>
+        <v>-2.63</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -1908,20 +1908,20 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>ORAGROUP TOGO (ORGT)</t>
+          <t>SOLIBRA CI (SLBC)</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D62" t="n">
-        <v>-12.37</v>
+        <v>-12.23</v>
       </c>
       <c r="E62" t="n">
-        <v>0.31</v>
+        <v>3.91</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -1932,20 +1932,20 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>CORIS BANK INTERNATIONAL (CBIBF)</t>
+          <t>ORAGROUP TOGO (ORGT)</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C63" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D63" t="n">
-        <v>-15.08</v>
+        <v>-12.37</v>
       </c>
       <c r="E63" t="n">
-        <v>2.86</v>
+        <v>0.31</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -1956,20 +1956,20 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>SOLIBRA CI (SLBC)</t>
+          <t>CORIS BANK INTERNATIONAL (CBIBF)</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C64" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D64" t="n">
-        <v>-16.14</v>
+        <v>-17.86</v>
       </c>
       <c r="E64" t="n">
-        <v>-3.79</v>
+        <v>-2.78</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>

</xml_diff>